<commit_message>
Problem solved: not reviewed
</commit_message>
<xml_diff>
--- a/Case/CS1/WACC.xlsx
+++ b/Case/CS1/WACC.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28702"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/park-wanbae/Desktop/MFE/2018-1/FIN521/Case/CS1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanbaep2/Desktop/FIN521/Case/CS1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1460" windowWidth="24700" windowHeight="13500"/>
+    <workbookView xWindow="3580" yWindow="1460" windowWidth="24700" windowHeight="13500"/>
   </bookViews>
   <sheets>
     <sheet name="시트1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Debt / Value</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -72,28 +78,37 @@
   <si>
     <t>Tax Rate</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Market Risk Premium</t>
+  </si>
+  <si>
+    <t>WACC</t>
+  </si>
+  <si>
+    <t>Tax Rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="0.0%"/>
-    <numFmt numFmtId="177" formatCode="0.0000%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -131,10 +146,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -142,7 +157,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="기본" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -454,20 +469,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -478,7 +495,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0.05</v>
       </c>
@@ -489,7 +506,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -517,55 +534,67 @@
       <c r="I3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="K3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>0</v>
       </c>
       <c r="B4" s="3">
-        <f>A4 / (1 - A4)</f>
+        <f t="shared" ref="B4:B9" si="0">A4 / (1 - A4)</f>
         <v>0</v>
       </c>
       <c r="C4">
         <v>1.18</v>
       </c>
       <c r="D4" s="1">
-        <f>$B$2 + C4 * $A$2</f>
+        <f t="shared" ref="D4:D9" si="1">$B$2 + C4 * $A$2</f>
         <v>9.6500000000000002E-2</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" s="5">
-        <f>C4 + B4 * (C4 - E4)</f>
+        <f t="shared" ref="F4:F9" si="2">C4 + B4 * (C4 - E4)</f>
         <v>1.18</v>
       </c>
       <c r="G4" s="1">
-        <f>$B$2 + E4 * $A$2</f>
+        <f t="shared" ref="G4:H9" si="3">$B$2 + E4 * $A$2</f>
         <v>3.7499999999999999E-2</v>
       </c>
       <c r="H4" s="1">
-        <f>$B$2 + F4 * $A$2</f>
+        <f t="shared" si="3"/>
         <v>9.6500000000000002E-2</v>
       </c>
       <c r="I4" s="4">
         <f>A4 * G4 * (1 - $C$2) + (1 - A4) * H4</f>
         <v>9.6500000000000002E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="K4" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="L4" s="1">
+        <v>6.9708000000000006E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>0.05</v>
       </c>
       <c r="B5" s="3">
-        <f>A5 / (1 - A5)</f>
+        <f t="shared" si="0"/>
         <v>5.2631578947368425E-2</v>
       </c>
       <c r="C5">
         <v>1.18</v>
       </c>
       <c r="D5" s="1">
-        <f>$B$2 + C5 * $A$2</f>
+        <f t="shared" si="1"/>
         <v>9.6500000000000002E-2</v>
       </c>
       <c r="E5">
@@ -573,35 +602,41 @@
         <v>2.0000000000000004E-2</v>
       </c>
       <c r="F5" s="5">
-        <f>C5 + B5 * (C5 - E5)</f>
+        <f t="shared" si="2"/>
         <v>1.2410526315789474</v>
       </c>
       <c r="G5" s="1">
-        <f>$B$2 + E5 * $A$2</f>
+        <f t="shared" si="3"/>
         <v>3.85E-2</v>
       </c>
       <c r="H5" s="1">
-        <f>$B$2 + F5 * $A$2</f>
+        <f t="shared" si="3"/>
         <v>9.9552631578947365E-2</v>
       </c>
       <c r="I5" s="4">
-        <f t="shared" ref="I5:I9" si="0">A5 * G5 * (1 - $C$2) + (1 - A5) * H5</f>
+        <f t="shared" ref="I5:I9" si="4">A5 * G5 * (1 - $C$2) + (1 - A5) * H5</f>
         <v>9.5729999999999996E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="K5" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="L5" s="1">
+        <v>8.1444000000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>0.1</v>
       </c>
       <c r="B6" s="3">
-        <f>A6 / (1 - A6)</f>
+        <f t="shared" si="0"/>
         <v>0.11111111111111112</v>
       </c>
       <c r="C6">
         <v>1.18</v>
       </c>
       <c r="D6" s="1">
-        <f>$B$2 + C6 * $A$2</f>
+        <f t="shared" si="1"/>
         <v>9.6500000000000002E-2</v>
       </c>
       <c r="E6">
@@ -609,35 +644,41 @@
         <v>4.0000000000000008E-2</v>
       </c>
       <c r="F6" s="5">
-        <f>C6 + B6 * (C6 - E6)</f>
+        <f t="shared" si="2"/>
         <v>1.3066666666666666</v>
       </c>
       <c r="G6" s="1">
-        <f>$B$2 + E6 * $A$2</f>
+        <f t="shared" si="3"/>
         <v>3.95E-2</v>
       </c>
       <c r="H6" s="1">
-        <f>$B$2 + F6 * $A$2</f>
+        <f t="shared" si="3"/>
         <v>0.10283333333333333</v>
       </c>
       <c r="I6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9.4920000000000004E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="K6" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="L6" s="1">
+        <v>9.3179999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>0.15</v>
       </c>
       <c r="B7" s="3">
-        <f>A7 / (1 - A7)</f>
+        <f t="shared" si="0"/>
         <v>0.17647058823529413</v>
       </c>
       <c r="C7">
         <v>1.18</v>
       </c>
       <c r="D7" s="1">
-        <f>$B$2 + C7 * $A$2</f>
+        <f t="shared" si="1"/>
         <v>9.6500000000000002E-2</v>
       </c>
       <c r="E7">
@@ -645,35 +686,41 @@
         <v>0.06</v>
       </c>
       <c r="F7" s="5">
-        <f>C7 + B7 * (C7 - E7)</f>
+        <f t="shared" si="2"/>
         <v>1.3776470588235292</v>
       </c>
       <c r="G7" s="1">
-        <f>$B$2 + E7 * $A$2</f>
+        <f t="shared" si="3"/>
         <v>4.0500000000000001E-2</v>
       </c>
       <c r="H7" s="1">
-        <f>$B$2 + F7 * $A$2</f>
+        <f t="shared" si="3"/>
         <v>0.10638235294117646</v>
       </c>
       <c r="I7" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9.4069999999999987E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="K7" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.104916</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>0.2</v>
       </c>
       <c r="B8" s="3">
-        <f>A8 / (1 - A8)</f>
+        <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
       <c r="C8">
         <v>1.18</v>
       </c>
       <c r="D8" s="1">
-        <f>$B$2 + C8 * $A$2</f>
+        <f t="shared" si="1"/>
         <v>9.6500000000000002E-2</v>
       </c>
       <c r="E8">
@@ -681,55 +728,154 @@
         <v>8.0000000000000016E-2</v>
       </c>
       <c r="F8" s="5">
-        <f>C8 + B8 * (C8 - E8)</f>
+        <f t="shared" si="2"/>
         <v>1.4549999999999998</v>
       </c>
       <c r="G8" s="1">
-        <f>$B$2 + E8 * $A$2</f>
+        <f t="shared" si="3"/>
         <v>4.1500000000000002E-2</v>
       </c>
       <c r="H8" s="1">
-        <f>$B$2 + F8 * $A$2</f>
+        <f t="shared" si="3"/>
         <v>0.11024999999999999</v>
       </c>
       <c r="I8" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9.3179999999999999E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="K8" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.11665200000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>0.25</v>
       </c>
       <c r="B9" s="3">
-        <f>A9 / (1 - A9)</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="C9">
         <v>1.18</v>
       </c>
       <c r="D9" s="1">
-        <f>$B$2 + C9 * $A$2</f>
+        <f t="shared" si="1"/>
         <v>9.6500000000000002E-2</v>
       </c>
       <c r="E9">
         <v>0.1</v>
       </c>
       <c r="F9" s="5">
-        <f>C9 + B9 * (C9 - E9)</f>
+        <f t="shared" si="2"/>
         <v>1.5399999999999998</v>
       </c>
       <c r="G9" s="1">
-        <f>$B$2 + E9 * $A$2</f>
+        <f t="shared" si="3"/>
         <v>4.2499999999999996E-2</v>
       </c>
       <c r="H9" s="1">
-        <f>$B$2 + F9 * $A$2</f>
+        <f t="shared" si="3"/>
         <v>0.11449999999999999</v>
       </c>
       <c r="I9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>9.2249999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K11" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="L11" s="1">
+        <v>9.3594999999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K12" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="L12" s="1">
+        <v>9.3511999999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K13" s="2">
+        <v>0.37</v>
+      </c>
+      <c r="L13" s="1">
+        <v>9.3428999999999998E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K14" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="L14" s="1">
+        <v>9.3345999999999998E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K15" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="L15" s="1">
+        <v>9.3262999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K16" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="L16" s="1">
+        <v>9.3179999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="K17" s="2">
+        <v>0.41</v>
+      </c>
+      <c r="L17" s="1">
+        <v>9.3096999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="K18" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="L18" s="1">
+        <v>9.3013999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="K19" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="L19" s="1">
+        <v>9.2931E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="K20" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="L20" s="1">
+        <v>9.2848E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="11:12" x14ac:dyDescent="0.2">
+      <c r="K21" s="2">
+        <v>0.45</v>
+      </c>
+      <c r="L21" s="1">
+        <v>9.2765E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>